<commit_message>
use `AbilityValues` instead of `AbilitySpecial`
</commit_message>
<xml_diff>
--- a/excels/lua_abilities.xlsx
+++ b/excels/lua_abilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\dota-ts-template\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\x-template\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84CFFE6-BB14-4023-B0D9-DBFBC36E0ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FEFE69-1707-46F8-B823-9B3F01E5DFB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="23254" windowHeight="12724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,54 +90,10 @@
     <t>AbilityManaCost</t>
   </si>
   <si>
-    <t>01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>如果需要更多的键可以自己加，会自动生成为var_01这样的格式，var_type kv生成器会自行判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>item_kv_generator_test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.1 0.2 0.3 0.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1 1 2 3 4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -190,12 +146,45 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AbilitySpecial[{]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ability_lua</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbilityValues[{]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>damage 0.1 0.2 0.3 0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -524,12 +513,12 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -542,41 +531,38 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
       <c r="Q1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="R1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="S1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="T1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="U1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="V1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="W1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="X1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -587,34 +573,34 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="N2" t="s">
         <v>12</v>
@@ -647,35 +633,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>